<commit_message>
Update spreadsheet for dozenal.
</commit_message>
<xml_diff>
--- a/assets/Starlendar.xlsx
+++ b/assets/Starlendar.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Decimal" sheetId="1" r:id="rId1"/>
+    <sheet name="Dozenal" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Q1</t>
   </si>
@@ -218,6 +217,21 @@
       </rPr>
       <t>rchday (U5)</t>
     </r>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>1X</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>Ultra days</t>
   </si>
 </sst>
 </file>
@@ -708,7 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -1222,24 +1236,516 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.08984375" customWidth="1"/>
+    <col min="2" max="16" width="4.6328125" customWidth="1"/>
+    <col min="17" max="17" width="0.54296875" customWidth="1"/>
+    <col min="18" max="18" width="12.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2"/>
+      <c r="B1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="12"/>
+    </row>
+    <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="13"/>
+    </row>
+    <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="13"/>
+    </row>
+    <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="14"/>
+    </row>
+    <row r="6" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>7</v>
+      </c>
+      <c r="D7" s="5">
+        <v>11</v>
+      </c>
+      <c r="E7" s="5">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5">
+        <v>21</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>7</v>
+      </c>
+      <c r="I7" s="6">
+        <v>11</v>
+      </c>
+      <c r="J7" s="6">
+        <v>17</v>
+      </c>
+      <c r="K7" s="6">
+        <v>21</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
+        <v>7</v>
+      </c>
+      <c r="N7" s="7">
+        <v>11</v>
+      </c>
+      <c r="O7" s="7">
+        <v>17</v>
+      </c>
+      <c r="P7" s="7">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5">
+        <v>22</v>
+      </c>
+      <c r="G8" s="6">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>8</v>
+      </c>
+      <c r="I8" s="6">
+        <v>12</v>
+      </c>
+      <c r="J8" s="6">
+        <v>18</v>
+      </c>
+      <c r="K8" s="6">
+        <v>22</v>
+      </c>
+      <c r="L8" s="7">
+        <v>2</v>
+      </c>
+      <c r="M8" s="7">
+        <v>8</v>
+      </c>
+      <c r="N8" s="7">
+        <v>12</v>
+      </c>
+      <c r="O8" s="7">
+        <v>18</v>
+      </c>
+      <c r="P8" s="7">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5">
+        <v>23</v>
+      </c>
+      <c r="G9" s="6">
+        <v>3</v>
+      </c>
+      <c r="H9" s="6">
+        <v>9</v>
+      </c>
+      <c r="I9" s="6">
+        <v>13</v>
+      </c>
+      <c r="J9" s="6">
+        <v>19</v>
+      </c>
+      <c r="K9" s="6">
+        <v>23</v>
+      </c>
+      <c r="L9" s="7">
+        <v>3</v>
+      </c>
+      <c r="M9" s="7">
+        <v>9</v>
+      </c>
+      <c r="N9" s="7">
+        <v>13</v>
+      </c>
+      <c r="O9" s="7">
+        <v>19</v>
+      </c>
+      <c r="P9" s="7">
+        <v>23</v>
+      </c>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="5">
+        <v>14</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="5">
+        <v>24</v>
+      </c>
+      <c r="G10" s="6">
+        <v>4</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="6">
+        <v>14</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="6">
+        <v>24</v>
+      </c>
+      <c r="L10" s="7">
+        <v>4</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="7">
+        <v>14</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="7">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="5">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5">
+        <v>25</v>
+      </c>
+      <c r="G11" s="6">
+        <v>5</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="6">
+        <v>15</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="6">
+        <v>25</v>
+      </c>
+      <c r="L11" s="7">
+        <v>5</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="7">
+        <v>15</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="7">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5">
+        <v>26</v>
+      </c>
+      <c r="G12" s="6">
+        <v>6</v>
+      </c>
+      <c r="H12" s="6">
+        <v>10</v>
+      </c>
+      <c r="I12" s="6">
+        <v>16</v>
+      </c>
+      <c r="J12" s="6">
+        <v>20</v>
+      </c>
+      <c r="K12" s="6">
+        <v>26</v>
+      </c>
+      <c r="L12" s="7">
+        <v>6</v>
+      </c>
+      <c r="M12" s="7">
+        <v>10</v>
+      </c>
+      <c r="N12" s="7">
+        <v>16</v>
+      </c>
+      <c r="O12" s="7">
+        <v>20</v>
+      </c>
+      <c r="P12" s="7">
+        <v>26</v>
+      </c>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="16">
+    <mergeCell ref="R2:R5"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:P4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="L5:P5"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Replace Sumday with Zingday.
</commit_message>
<xml_diff>
--- a/assets/Starlendar.xlsx
+++ b/assets/Starlendar.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Decimal" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t>Q1</t>
   </si>
@@ -30,24 +30,6 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>Starday</t>
-  </si>
-  <si>
-    <t>Topday</t>
-  </si>
-  <si>
-    <t>Aceday</t>
-  </si>
-  <si>
-    <t>Rolday</t>
-  </si>
-  <si>
-    <t>Sumday</t>
-  </si>
-  <si>
-    <t>Funday</t>
-  </si>
-  <si>
     <t>Alba (Jan)</t>
   </si>
   <si>
@@ -100,9 +82,6 @@
   </si>
   <si>
     <t>Leapday (U6)</t>
-  </si>
-  <si>
-    <t>Ultra days AKA intercalary days</t>
   </si>
   <si>
     <r>
@@ -266,6 +245,24 @@
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Starday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Topday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aceday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rolday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zingday</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Funday</t>
   </si>
 </sst>
 </file>
@@ -432,6 +429,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,18 +461,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,7 +766,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -782,148 +779,148 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="B1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
+      <c r="B2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="12"/>
+      <c r="R2" s="16"/>
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
       <c r="Q3" s="10"/>
-      <c r="R3" s="13"/>
+      <c r="R3" s="17"/>
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
       <c r="Q4" s="10"/>
-      <c r="R4" s="13"/>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
+      <c r="B5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
       <c r="Q5" s="10"/>
-      <c r="R5" s="14"/>
+      <c r="R5" s="18"/>
     </row>
     <row r="6" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -972,12 +969,12 @@
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B8" s="5">
         <v>2</v>
@@ -1026,12 +1023,12 @@
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
@@ -1080,12 +1077,12 @@
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
@@ -1134,12 +1131,12 @@
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
@@ -1188,12 +1185,12 @@
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5">
         <v>6</v>
@@ -1242,18 +1239,18 @@
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1284,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1298,148 +1295,148 @@
   <sheetData>
     <row r="1" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="B1" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
       <c r="Q1" s="9"/>
       <c r="R1" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
+      <c r="B2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="12"/>
+      <c r="R2" s="16"/>
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
       <c r="Q3" s="10"/>
-      <c r="R3" s="13"/>
+      <c r="R3" s="17"/>
     </row>
     <row r="4" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
       <c r="Q4" s="10"/>
-      <c r="R4" s="13"/>
+      <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
+      <c r="B5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
       <c r="Q5" s="10"/>
-      <c r="R5" s="14"/>
+      <c r="R5" s="18"/>
     </row>
     <row r="6" spans="1:18" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -1488,12 +1485,12 @@
       </c>
       <c r="Q7" s="1"/>
       <c r="R7" s="8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B8" s="5">
         <v>2</v>
@@ -1542,12 +1539,12 @@
       </c>
       <c r="Q8" s="1"/>
       <c r="R8" s="8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
@@ -1596,24 +1593,24 @@
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B10" s="5">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D10" s="5">
         <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F10" s="5">
         <v>24</v>
@@ -1622,13 +1619,13 @@
         <v>4</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="I10" s="6">
         <v>14</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="K10" s="6">
         <v>24</v>
@@ -1637,37 +1634,37 @@
         <v>4</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="N10" s="7">
         <v>14</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="P10" s="7">
         <v>24</v>
       </c>
       <c r="Q10" s="1"/>
       <c r="R10" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D11" s="5">
         <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F11" s="5">
         <v>25</v>
@@ -1676,13 +1673,13 @@
         <v>5</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I11" s="6">
         <v>15</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="K11" s="6">
         <v>25</v>
@@ -1691,25 +1688,25 @@
         <v>5</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="N11" s="7">
         <v>15</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="P11" s="7">
         <v>25</v>
       </c>
       <c r="Q11" s="1"/>
       <c r="R11" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="16" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B12" s="5">
         <v>6</v>
@@ -1758,22 +1755,28 @@
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="4.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
     <mergeCell ref="R2:R5"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="G3:K3"/>
@@ -1784,12 +1787,6 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="G5:K5"/>
     <mergeCell ref="L5:P5"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1800,209 +1797,209 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="11.6328125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="19" customWidth="1"/>
+    <col min="1" max="3" width="11.6328125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" style="12" customWidth="1"/>
     <col min="7" max="7" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="12">
+        <v>2011</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
+        <v>2012</v>
+      </c>
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
+        <v>2013</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
+        <v>2014</v>
+      </c>
+      <c r="B5" s="12">
+        <v>3</v>
+      </c>
+      <c r="C5" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
+        <v>2015</v>
+      </c>
+      <c r="B6" s="12">
+        <v>4</v>
+      </c>
+      <c r="C6" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
+        <v>2016</v>
+      </c>
+      <c r="B7" s="12">
+        <v>5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
+        <v>2017</v>
+      </c>
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
+        <v>2018</v>
+      </c>
+      <c r="B9" s="12">
+        <v>7</v>
+      </c>
+      <c r="C9" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="12">
+        <v>2019</v>
+      </c>
+      <c r="B10" s="12">
+        <v>8</v>
+      </c>
+      <c r="C10" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="12">
+        <v>2020</v>
+      </c>
+      <c r="B11" s="12">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12">
+        <v>9</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="12">
+        <v>2021</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="12">
+        <v>2022</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
+        <v>2023</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
+        <v>2024</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C15" s="12">
+        <v>13</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="21" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="19">
-        <v>2011</v>
-      </c>
-      <c r="B2" s="19">
-        <v>0</v>
-      </c>
-      <c r="C2" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="19">
-        <v>2012</v>
-      </c>
-      <c r="B3" s="19">
-        <v>1</v>
-      </c>
-      <c r="C3" s="19">
-        <v>1</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="19">
-        <v>2013</v>
-      </c>
-      <c r="B4" s="19">
-        <v>2</v>
-      </c>
-      <c r="C4" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="19">
-        <v>2014</v>
-      </c>
-      <c r="B5" s="19">
-        <v>3</v>
-      </c>
-      <c r="C5" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19">
-        <v>2015</v>
-      </c>
-      <c r="B6" s="19">
-        <v>4</v>
-      </c>
-      <c r="C6" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="19">
-        <v>2016</v>
-      </c>
-      <c r="B7" s="19">
-        <v>5</v>
-      </c>
-      <c r="C7" s="19">
-        <v>5</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="19">
-        <v>2017</v>
-      </c>
-      <c r="B8" s="19">
-        <v>6</v>
-      </c>
-      <c r="C8" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="19">
-        <v>2018</v>
-      </c>
-      <c r="B9" s="19">
-        <v>7</v>
-      </c>
-      <c r="C9" s="19">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19">
-        <v>2019</v>
-      </c>
-      <c r="B10" s="19">
-        <v>8</v>
-      </c>
-      <c r="C10" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19">
-        <v>2020</v>
-      </c>
-      <c r="B11" s="19">
-        <v>9</v>
-      </c>
-      <c r="C11" s="19">
-        <v>9</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19">
-        <v>2021</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19">
-        <v>2022</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="19">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="19">
-        <v>2023</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="19">
-        <v>2024</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="19">
-        <v>13</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>49</v>
+      <c r="B16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>